<commit_message>
updated spreadsheet with reworked db plan
</commit_message>
<xml_diff>
--- a/app planning.xlsx
+++ b/app planning.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bquan\Documents\Projects\transaction_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bquan\Documents\Projects\PFiT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3772C7BD-248B-4A5C-AA82-65FF3E57400D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922A1BAD-9D3B-4730-9E9E-D5694DBBF045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E6C4F384-4C64-4F4C-8CA7-8BD591700B12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{E6C4F384-4C64-4F4C-8CA7-8BD591700B12}"/>
   </bookViews>
   <sheets>
     <sheet name="architecture" sheetId="1" r:id="rId1"/>
     <sheet name="database" sheetId="2" r:id="rId2"/>
     <sheet name="database2" sheetId="5" r:id="rId3"/>
-    <sheet name="flexible cat UI" sheetId="4" r:id="rId4"/>
-    <sheet name="hypothetical data" sheetId="3" r:id="rId5"/>
+    <sheet name="database3" sheetId="6" r:id="rId4"/>
+    <sheet name="flexible cat UI" sheetId="4" r:id="rId5"/>
+    <sheet name="hypothetical data" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="153">
   <si>
     <t>Table</t>
   </si>
@@ -379,9 +379,6 @@
     <t>Menu Category</t>
   </si>
   <si>
-    <t>trx_id</t>
-  </si>
-  <si>
     <t>parent_id</t>
   </si>
   <si>
@@ -401,12 +398,6 @@
   </si>
   <si>
     <t>isLeaf</t>
-  </si>
-  <si>
-    <t>Transaction Category Mapping</t>
-  </si>
-  <si>
-    <t>maping_id</t>
   </si>
   <si>
     <t>plan_id</t>
@@ -426,6 +417,94 @@
   </si>
   <si>
     <t>Parent values will have parent_id value of -1</t>
+  </si>
+  <si>
+    <t>Analytic Plan</t>
+  </si>
+  <si>
+    <t>default 1, represents the number of categories used in the plan. Has a max limit of X</t>
+  </si>
+  <si>
+    <t>plan_name</t>
+  </si>
+  <si>
+    <t>plan_desc</t>
+  </si>
+  <si>
+    <t>pk. In order to make the number of category per plan flexible, this table denormalizes plan_id</t>
+  </si>
+  <si>
+    <t>plan_denorm_id</t>
+  </si>
+  <si>
+    <t>Table:</t>
+  </si>
+  <si>
+    <t>Columns:</t>
+  </si>
+  <si>
+    <t>category_code</t>
+  </si>
+  <si>
+    <t>category_description</t>
+  </si>
+  <si>
+    <t>category_type</t>
+  </si>
+  <si>
+    <t>table containing all the unique categories that can be used in an analytic plan. A category is a value set that  will contain values</t>
+  </si>
+  <si>
+    <t>Thought:</t>
+  </si>
+  <si>
+    <t>simple_category_values</t>
+  </si>
+  <si>
+    <t>cat_value_id</t>
+  </si>
+  <si>
+    <t>once assigned, cannot change since there will be dedicated tables per type</t>
+  </si>
+  <si>
+    <t>value_code</t>
+  </si>
+  <si>
+    <t>value_description</t>
+  </si>
+  <si>
+    <t>menu_category_values</t>
+  </si>
+  <si>
+    <t>is_child</t>
+  </si>
+  <si>
+    <t>hierarchy_category_values</t>
+  </si>
+  <si>
+    <t>category_set</t>
+  </si>
+  <si>
+    <t>position_id</t>
+  </si>
+  <si>
+    <t>Row-flattened structure to store hierarchy of values</t>
+  </si>
+  <si>
+    <t>references the position_id if this record is a child row.
+Is null for the root value</t>
+  </si>
+  <si>
+    <t>separate id to track the position of the value (versus using the PK). Numerical value should reflect the order of the position relative to the parent</t>
+  </si>
+  <si>
+    <t>Distance from the root. Starts at 1 for the root. Needs to update accordinly based on the assignment. This may not be needed since this is a row-flattened structure…but it'd be convenient</t>
+  </si>
+  <si>
+    <t>references the cat_value_id of a parent value when this row is a child value</t>
+  </si>
+  <si>
+    <t>username of the owner</t>
   </si>
 </sst>
 </file>
@@ -496,21 +575,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -850,34 +927,34 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" customWidth="1"/>
+    <col min="7" max="7" width="38.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>57</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -887,16 +964,16 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="6"/>
       <c r="E3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
@@ -917,19 +994,19 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +1023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -957,7 +1034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -968,7 +1045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -985,7 +1062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -996,7 +1073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1035,54 +1112,54 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1095,11 +1172,11 @@
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1112,9 +1189,9 @@
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1127,9 +1204,9 @@
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1140,7 +1217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1154,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1168,7 +1245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1185,7 +1262,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1202,7 +1279,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1213,7 +1290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1227,7 +1304,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1241,7 +1318,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1252,188 +1329,188 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1452,106 +1529,107 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8671A98D-06A2-478F-A122-360846259519}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="35" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="8" t="s">
+    <row r="1" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="K1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="H6" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="K8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1568,10 +1646,13 @@
         <v>105</v>
       </c>
       <c r="N9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1588,10 +1669,10 @@
         <v>106</v>
       </c>
       <c r="N10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1605,233 +1686,242 @@
         <v>107</v>
       </c>
       <c r="N11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>108</v>
       </c>
       <c r="N12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>109</v>
       </c>
       <c r="N13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="K15" t="s">
+        <v>116</v>
+      </c>
+      <c r="N15" t="s">
+        <v>109</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1848,6 +1938,164 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6F602E-4BE3-4929-BA5A-3FCC6DC5D164}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="33.88671875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773B826D-E19C-45BE-8548-B42F8BF2C210}">
   <dimension ref="A1:O14"/>
   <sheetViews>
@@ -1855,14 +2103,14 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1891,7 +2139,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1911,7 +2159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1931,7 +2179,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
         <v>39</v>
       </c>
@@ -1945,7 +2193,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I5" t="s">
         <v>39</v>
       </c>
@@ -1962,27 +2210,27 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.03</v>
       </c>
@@ -1992,22 +2240,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A257E6A-7A31-4B40-A8A2-4F8901B4B547}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>38</v>
       </c>
@@ -2020,19 +2268,8 @@
       <c r="F1" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -2051,19 +2288,8 @@
       <c r="F2" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -2082,19 +2308,8 @@
       <c r="F3" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -2113,225 +2328,6 @@
       <c r="F4" t="s">
         <v>101</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-    </row>
-    <row r="17" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-    </row>
-    <row r="18" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-    </row>
-    <row r="19" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-    </row>
-    <row r="20" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>